<commit_message>
Multiples validaciones para 3 secciones:
</commit_message>
<xml_diff>
--- a/Test/TemplatesTest/WebService1Test/ObtenerProducto/ObtenerProducto.xlsx
+++ b/Test/TemplatesTest/WebService1Test/ObtenerProducto/ObtenerProducto.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>string</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Caso4</t>
   </si>
   <si>
-    <t>HJ5KS9876234DD342</t>
-  </si>
-  <si>
     <t>Caso5</t>
   </si>
   <si>
@@ -55,6 +52,15 @@
   </si>
   <si>
     <t>HJ5KS987dddDD3434</t>
+  </si>
+  <si>
+    <t>${NULL}</t>
+  </si>
+  <si>
+    <t>Caso6</t>
+  </si>
+  <si>
+    <t>${EMPTY}</t>
   </si>
 </sst>
 </file>
@@ -372,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I7" sqref="I7:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +391,7 @@
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -399,30 +405,36 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
+      <c r="H2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primera aproximacion de caso de borde
</commit_message>
<xml_diff>
--- a/Test/TemplatesTest/WebService1Test/ObtenerProducto/ObtenerProducto.xlsx
+++ b/Test/TemplatesTest/WebService1Test/ObtenerProducto/ObtenerProducto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>Caso1</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>${EMPTY}</t>
+  </si>
+  <si>
+    <t>xsd:string</t>
   </si>
 </sst>
 </file>
@@ -381,11 +381,12 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:J8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -393,48 +394,48 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>